<commit_message>
Will only create LinkedIn sheet if cell in column reads unavailable
</commit_message>
<xml_diff>
--- a/Test.xlsx
+++ b/Test.xlsx
@@ -10,7 +10,7 @@
     <sheet name="Linkedin Only" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
-  <calcPr calcId="191028" fullCalcOnLoad="1"/>
+  <calcPr calcId="0" fullCalcOnLoad="1"/>
 </workbook>
 </file>
 
@@ -446,7 +446,7 @@
   <dimension ref="A1:Z1000"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E7" sqref="E7"/>
+      <selection activeCell="G9" sqref="G9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="16"/>

</xml_diff>